<commit_message>
[ENH] pabi_utils, adding subtotal
</commit_message>
<xml_diff>
--- a/pabi_budget_plan/xlsx_template/budget_plan_personnel_20180530.xlsx
+++ b/pabi_budget_plan/xlsx_template/budget_plan_personnel_20180530.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>สก.</t>
   </si>
@@ -1265,7 +1265,7 @@
       <selection activeCell="O15" sqref="O15"/>
       <selection pane="topRight" activeCell="O15" sqref="O15"/>
       <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -2088,14 +2088,14 @@
       </c>
       <c r="C11" s="35" t="str">
         <f>IF($D11="","",VLOOKUP(LEFT($D11,1),TAB_List!$B$5:$F$12,2,FALSE))</f>
-        <v>ศช.</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>42</v>
+        <v>ศว.</v>
+      </c>
+      <c r="D11" s="34">
+        <v>309999</v>
       </c>
       <c r="E11" s="34" t="str">
         <f t="shared" si="2"/>
-        <v>งบบุคลากรเงินเดือนและสวัสดิการ ศช.</v>
+        <v>งบบุคลากรเงินเดือนและสวัสดิการ ศว.</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>33</v>
@@ -7330,6 +7330,7 @@
       <c r="F12" s="48"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="7OB1+t5m3VkVrUO5xbAEiVEZ+rFijDn2AWh5Dg33TZvARPst3xwhn/WnqWZkO2MNxGTtycw5XtfLVK2KhBUoGg==" saltValue="sCo2r4zio24TobQstq4ofQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>